<commit_message>
markdown package initial split and test
</commit_message>
<xml_diff>
--- a/test/testfiles/iGEM_LUDOX_OD_calibration_2018.xlsx
+++ b/test/testfiles/iGEM_LUDOX_OD_calibration_2018.xlsx
@@ -1,12 +1,12 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="9560" yWindow="5640" windowWidth="26040" windowHeight="14940" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Data Reporting" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Data Reporting" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="181029" fullCalcOnLoad="1"/>
@@ -595,7 +595,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
@@ -758,6 +758,6 @@
     <mergeCell ref="C4:D4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="anysvml"/>
+  <legacyDrawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="anysvml"/>
 </worksheet>
 </file>
</xml_diff>